<commit_message>
Spearman's rank corr coeff
</commit_message>
<xml_diff>
--- a/coldpool_recovery.xlsx
+++ b/coldpool_recovery.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deszoeks/Projects/ATOMIC/coldpools/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3088DD3-8BA3-7F49-9CBD-FC253E032F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB582248-EE1B-1146-B5FB-C3EF4739D53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="1780" windowWidth="24000" windowHeight="14820" activeTab="3" xr2:uid="{57AE2C8F-3C7E-8F4E-937F-AEC883ABBC77}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet2.1" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,8 +38,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="73">
   <si>
     <t>lambda_WV</t>
   </si>
@@ -299,6 +321,9 @@
   <si>
     <t>ΔT Ranking</t>
   </si>
+  <si>
+    <t>Spearman's rank correlation coefficient</t>
+  </si>
 </sst>
 </file>
 
@@ -306,7 +331,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -465,26 +490,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
@@ -525,43 +549,41 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="4" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +621,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C444F7B-DD4E-F435-4CF3-D1F5D2A481DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -670,7 +692,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FE4E392-5CB5-5DCC-B944-3FFE1D39BFF0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -741,7 +763,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E45CB2-80E0-6E70-C726-2D44F4FC117E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -817,7 +839,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C444F7B-DD4E-F435-4CF3-D1F5D2A481DC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -888,7 +910,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68E45CB2-80E0-6E70-C726-2D44F4FC117E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1310,21 +1332,21 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="11" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:13" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="12"/>
-      <c r="J3" s="11" t="s">
+      <c r="G3" s="11"/>
+      <c r="J3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1336,7 +1358,7 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" s="13"/>
+      <c r="E4" s="12"/>
       <c r="F4" s="4"/>
       <c r="G4" s="9"/>
       <c r="H4" s="5"/>
@@ -1354,13 +1376,13 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>15.8193</v>
       </c>
       <c r="F5" s="1">
         <v>17.5594</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="7">
         <v>55</v>
       </c>
       <c r="H5" s="6">
@@ -1394,13 +1416,13 @@
       <c r="D6">
         <v>3</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>22.813600000000001</v>
       </c>
       <c r="F6" s="1">
         <v>12.176</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="7">
         <v>7</v>
       </c>
       <c r="H6" s="6">
@@ -1434,13 +1456,13 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>24.6111</v>
       </c>
       <c r="F7" s="1">
         <v>11.2867</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="7">
         <v>4</v>
       </c>
       <c r="H7" s="6">
@@ -1470,13 +1492,13 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>64.723600000000005</v>
       </c>
       <c r="F8" s="1">
         <v>4.2918000000000003</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="7">
         <v>8</v>
       </c>
       <c r="H8" s="6">
@@ -1510,13 +1532,13 @@
       <c r="D9">
         <v>6</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>43.758600000000001</v>
       </c>
       <c r="F9" s="1">
         <v>6.3479999999999999</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="7">
         <v>23</v>
       </c>
       <c r="H9" s="6">
@@ -1550,13 +1572,13 @@
       <c r="D10">
         <v>7</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>115.23860000000001</v>
       </c>
       <c r="F10" s="1">
         <v>2.4104999999999999</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="7">
         <v>31</v>
       </c>
       <c r="H10" s="6">
@@ -1590,13 +1612,13 @@
       <c r="D11">
         <v>8</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>56.107599999999998</v>
       </c>
       <c r="F11" s="1">
         <v>4.9508000000000001</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="7">
         <v>20</v>
       </c>
       <c r="H11" s="6">
@@ -1630,13 +1652,13 @@
       <c r="D12">
         <v>9</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>41.937199999999997</v>
       </c>
       <c r="F12" s="1">
         <v>6.6237000000000004</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G12" s="7">
         <v>22</v>
       </c>
       <c r="H12" s="6">
@@ -1670,13 +1692,13 @@
       <c r="D13">
         <v>10</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <v>44.925699999999999</v>
       </c>
       <c r="F13" s="1">
         <v>6.1829999999999998</v>
       </c>
-      <c r="G13" s="10">
+      <c r="G13" s="7">
         <v>13</v>
       </c>
       <c r="H13" s="6">
@@ -1710,13 +1732,13 @@
       <c r="D14">
         <v>11</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>50.024900000000002</v>
       </c>
       <c r="F14" s="1">
         <v>5.5528000000000004</v>
       </c>
-      <c r="G14" s="10">
+      <c r="G14" s="7">
         <v>9</v>
       </c>
       <c r="H14" s="6">
@@ -1750,7 +1772,7 @@
       <c r="D15">
         <v>12</v>
       </c>
-      <c r="E15" s="13"/>
+      <c r="E15" s="12"/>
       <c r="F15" s="4"/>
       <c r="G15" s="9"/>
       <c r="H15" s="5"/>
@@ -1772,13 +1794,13 @@
       <c r="D16">
         <v>13</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>38.146099999999997</v>
       </c>
       <c r="F16" s="1">
         <v>7.2819000000000003</v>
       </c>
-      <c r="G16" s="10">
+      <c r="G16" s="7">
         <v>32</v>
       </c>
       <c r="H16" s="6">
@@ -1812,13 +1834,13 @@
       <c r="D17">
         <v>14</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>31.484200000000001</v>
       </c>
       <c r="F17" s="1">
         <v>8.8228000000000009</v>
       </c>
-      <c r="G17" s="10">
+      <c r="G17" s="7">
         <v>3</v>
       </c>
       <c r="H17" s="6">
@@ -1848,13 +1870,13 @@
       <c r="D18">
         <v>15</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>46.346600000000002</v>
       </c>
       <c r="F18" s="1">
         <v>5.9935</v>
       </c>
-      <c r="G18" s="10">
+      <c r="G18" s="7">
         <v>7</v>
       </c>
       <c r="H18" s="6">
@@ -1888,13 +1910,13 @@
       <c r="D19">
         <v>16</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>29.519300000000001</v>
       </c>
       <c r="F19" s="1">
         <v>9.41</v>
       </c>
-      <c r="G19" s="10">
+      <c r="G19" s="7">
         <v>10</v>
       </c>
       <c r="H19" s="6">
@@ -1946,7 +1968,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="20.5" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="29"/>
+    <col min="9" max="9" width="10.83203125" style="27"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1978,7 +2000,7 @@
       <c r="H2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="28" t="s">
         <v>20</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -1994,30 +2016,30 @@
       <c r="N2" s="3"/>
     </row>
     <row r="3" spans="1:14" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="12" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="H3" s="12"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11" t="s">
+      <c r="H3" s="11"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
@@ -2032,16 +2054,16 @@
       <c r="E4">
         <v>10</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="13">
         <v>15.8193</v>
       </c>
       <c r="G4" s="1">
         <v>17.5594</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="7">
         <v>55</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="30">
         <v>3.0499999999999999E-2</v>
       </c>
       <c r="J4" s="6">
@@ -2054,7 +2076,7 @@
         <v>35.451599999999999</v>
       </c>
       <c r="M4">
-        <f>L4/60</f>
+        <f t="shared" ref="M4:M17" si="0">L4/60</f>
         <v>0.59085999999999994</v>
       </c>
       <c r="N4">
@@ -2075,16 +2097,16 @@
       <c r="E5">
         <v>13</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="13">
         <v>22.813600000000001</v>
       </c>
       <c r="G5" s="1">
         <v>12.176</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="7">
         <v>7</v>
       </c>
-      <c r="I5" s="32">
+      <c r="I5" s="30">
         <v>1.66E-2</v>
       </c>
       <c r="J5" s="6">
@@ -2097,7 +2119,7 @@
         <v>3.0716000000000001</v>
       </c>
       <c r="M5">
-        <f>L5/60</f>
+        <f t="shared" si="0"/>
         <v>5.1193333333333334E-2</v>
       </c>
       <c r="N5">
@@ -2118,16 +2140,16 @@
       <c r="E6">
         <v>14</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="13">
         <v>24.6111</v>
       </c>
       <c r="G6" s="1">
         <v>11.2867</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6" s="7">
         <v>4</v>
       </c>
-      <c r="I6" s="32">
+      <c r="I6" s="30">
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="J6" s="6">
@@ -2140,7 +2162,7 @@
         <v>18</v>
       </c>
       <c r="M6" t="e">
-        <f>L6/60</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2157,16 +2179,16 @@
       <c r="E7">
         <v>8</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="13">
         <v>64.723600000000005</v>
       </c>
       <c r="G7" s="1">
         <v>4.2918000000000003</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7" s="7">
         <v>8</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="30">
         <v>4.0500000000000001E-2</v>
       </c>
       <c r="J7" s="6">
@@ -2179,11 +2201,11 @@
         <v>17.647400000000001</v>
       </c>
       <c r="M7">
-        <f>L7/60</f>
+        <f t="shared" si="0"/>
         <v>0.29412333333333335</v>
       </c>
       <c r="N7">
-        <f>G7/M7</f>
+        <f t="shared" ref="N7:N14" si="1">G7/M7</f>
         <v>14.591837891134105</v>
       </c>
     </row>
@@ -2200,16 +2222,16 @@
       <c r="E8">
         <v>4</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="13">
         <v>43.758600000000001</v>
       </c>
       <c r="G8" s="1">
         <v>6.3479999999999999</v>
       </c>
-      <c r="H8" s="10">
+      <c r="H8" s="7">
         <v>23</v>
       </c>
-      <c r="I8" s="32">
+      <c r="I8" s="30">
         <v>8.2400000000000001E-2</v>
       </c>
       <c r="J8" s="6">
@@ -2222,11 +2244,11 @@
         <v>24.612200000000001</v>
       </c>
       <c r="M8">
-        <f>L8/60</f>
+        <f t="shared" si="0"/>
         <v>0.41020333333333336</v>
       </c>
       <c r="N8">
-        <f>G8/M8</f>
+        <f t="shared" si="1"/>
         <v>15.475252110741826</v>
       </c>
     </row>
@@ -2243,16 +2265,16 @@
       <c r="E9">
         <v>3</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <v>115.23860000000001</v>
       </c>
       <c r="G9" s="1">
         <v>2.4104999999999999</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9" s="7">
         <v>31</v>
       </c>
-      <c r="I9" s="32">
+      <c r="I9" s="30">
         <v>0.1328</v>
       </c>
       <c r="J9" s="6">
@@ -2265,11 +2287,11 @@
         <v>25.7301</v>
       </c>
       <c r="M9">
-        <f>L9/60</f>
+        <f t="shared" si="0"/>
         <v>0.42883500000000002</v>
       </c>
       <c r="N9">
-        <f>G9/M9</f>
+        <f t="shared" si="1"/>
         <v>5.6210430585190103</v>
       </c>
     </row>
@@ -2286,16 +2308,16 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="13">
         <v>56.107599999999998</v>
       </c>
       <c r="G10" s="1">
         <v>4.9508000000000001</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="7">
         <v>20</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="30">
         <v>0.34160000000000001</v>
       </c>
       <c r="J10" s="6">
@@ -2308,11 +2330,11 @@
         <v>15.8201</v>
       </c>
       <c r="M10">
-        <f>L10/60</f>
+        <f t="shared" si="0"/>
         <v>0.26366833333333334</v>
       </c>
       <c r="N10">
-        <f>G10/M10</f>
+        <f t="shared" si="1"/>
         <v>18.776619616816582</v>
       </c>
     </row>
@@ -2329,16 +2351,16 @@
       <c r="E11">
         <v>7</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="13">
         <v>41.937199999999997</v>
       </c>
       <c r="G11" s="1">
         <v>6.6237000000000004</v>
       </c>
-      <c r="H11" s="10">
+      <c r="H11" s="7">
         <v>22</v>
       </c>
-      <c r="I11" s="32">
+      <c r="I11" s="30">
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="J11" s="6">
@@ -2351,11 +2373,11 @@
         <v>10.45</v>
       </c>
       <c r="M11">
-        <f>L11/60</f>
+        <f t="shared" si="0"/>
         <v>0.17416666666666666</v>
       </c>
       <c r="N11">
-        <f>G11/M11</f>
+        <f t="shared" si="1"/>
         <v>38.030813397129187</v>
       </c>
     </row>
@@ -2372,16 +2394,16 @@
       <c r="E12">
         <v>6</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="13">
         <v>44.925699999999999</v>
       </c>
       <c r="G12" s="1">
         <v>6.1829999999999998</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12" s="7">
         <v>13</v>
       </c>
-      <c r="I12" s="32">
+      <c r="I12" s="30">
         <v>5.7099999999999998E-2</v>
       </c>
       <c r="J12" s="6">
@@ -2394,11 +2416,11 @@
         <v>1.6933</v>
       </c>
       <c r="M12">
-        <f>L12/60</f>
+        <f t="shared" si="0"/>
         <v>2.8221666666666666E-2</v>
       </c>
       <c r="N12">
-        <f>G12/M12</f>
+        <f t="shared" si="1"/>
         <v>219.086989901376</v>
       </c>
     </row>
@@ -2415,16 +2437,16 @@
       <c r="E13">
         <v>9</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="13">
         <v>50.024900000000002</v>
       </c>
       <c r="G13" s="1">
         <v>5.5528000000000004</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13" s="7">
         <v>9</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="30">
         <v>3.5000000000000003E-2</v>
       </c>
       <c r="J13" s="6">
@@ -2437,11 +2459,11 @@
         <v>5.266</v>
       </c>
       <c r="M13">
-        <f>L13/60</f>
+        <f t="shared" si="0"/>
         <v>8.7766666666666673E-2</v>
       </c>
       <c r="N13">
-        <f>G13/M13</f>
+        <f t="shared" si="1"/>
         <v>63.267755412077477</v>
       </c>
     </row>
@@ -2458,16 +2480,16 @@
       <c r="E14">
         <v>5</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="13">
         <v>38.146099999999997</v>
       </c>
       <c r="G14" s="1">
         <v>7.2819000000000003</v>
       </c>
-      <c r="H14" s="10">
+      <c r="H14" s="7">
         <v>32</v>
       </c>
-      <c r="I14" s="32">
+      <c r="I14" s="30">
         <v>8.0699999999999994E-2</v>
       </c>
       <c r="J14" s="6">
@@ -2480,11 +2502,11 @@
         <v>10.397500000000001</v>
       </c>
       <c r="M14">
-        <f>L14/60</f>
+        <f t="shared" si="0"/>
         <v>0.17329166666666668</v>
       </c>
       <c r="N14">
-        <f>G14/M14</f>
+        <f t="shared" si="1"/>
         <v>42.021062755470062</v>
       </c>
     </row>
@@ -2501,16 +2523,16 @@
       <c r="E15">
         <v>11</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="13">
         <v>31.484200000000001</v>
       </c>
       <c r="G15" s="1">
         <v>8.8228000000000009</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15" s="7">
         <v>3</v>
       </c>
-      <c r="I15" s="32">
+      <c r="I15" s="30">
         <v>2.7400000000000001E-2</v>
       </c>
       <c r="J15" s="6">
@@ -2523,7 +2545,7 @@
         <v>18</v>
       </c>
       <c r="M15" t="e">
-        <f>L15/60</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -2540,16 +2562,16 @@
       <c r="E16">
         <v>12</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="13">
         <v>46.346600000000002</v>
       </c>
       <c r="G16" s="1">
         <v>5.9935</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16" s="7">
         <v>7</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16" s="30">
         <v>2.3900000000000001E-2</v>
       </c>
       <c r="J16" s="6">
@@ -2562,7 +2584,7 @@
         <v>1.0656000000000001</v>
       </c>
       <c r="M16">
-        <f>L16/60</f>
+        <f t="shared" si="0"/>
         <v>1.7760000000000001E-2</v>
       </c>
       <c r="N16">
@@ -2583,16 +2605,16 @@
       <c r="E17">
         <v>2</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="13">
         <v>29.519300000000001</v>
       </c>
       <c r="G17" s="1">
         <v>9.41</v>
       </c>
-      <c r="H17" s="10">
+      <c r="H17" s="7">
         <v>10</v>
       </c>
-      <c r="I17" s="32">
+      <c r="I17" s="30">
         <v>0.31929999999999997</v>
       </c>
       <c r="J17" s="6">
@@ -2605,7 +2627,7 @@
         <v>39.353900000000003</v>
       </c>
       <c r="M17">
-        <f>L17/60</f>
+        <f t="shared" si="0"/>
         <v>0.65589833333333336</v>
       </c>
       <c r="N17">
@@ -2636,32 +2658,32 @@
   <sheetData>
     <row r="1" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="27" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:8" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="18" t="s">
+      <c r="B3" s="37"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="18" t="s">
+      <c r="F3" s="37"/>
+      <c r="G3" s="17" t="s">
         <v>51</v>
       </c>
       <c r="H3" t="s">
@@ -2669,20 +2691,20 @@
       </c>
     </row>
     <row r="4" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>43868.520138888889</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="20">
+      <c r="C4" s="31"/>
+      <c r="D4" s="19">
         <v>3.3940000000000001</v>
       </c>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="F4" s="20">
+      <c r="F4" s="19">
         <v>8.25</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>14</v>
       </c>
       <c r="H4">
@@ -2690,20 +2712,20 @@
       </c>
     </row>
     <row r="5" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>43871.665972222225</v>
       </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="20">
+      <c r="C5" s="31"/>
+      <c r="D5" s="19">
         <v>2.6459999999999999</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="19">
         <v>4.84</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>13</v>
       </c>
       <c r="H5">
@@ -2711,20 +2733,20 @@
       </c>
     </row>
     <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
+      <c r="B6" s="22">
         <v>43869.433333333334</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="24">
+      <c r="C6" s="32"/>
+      <c r="D6" s="23">
         <v>1.3009999999999999</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="F6" s="24">
+      <c r="F6" s="23">
         <v>1.8520000000000001</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="24">
         <v>7</v>
       </c>
       <c r="H6">
@@ -2732,20 +2754,20 @@
       </c>
     </row>
     <row r="7" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
+      <c r="B7" s="22">
         <v>43859.568749999999</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="24">
+      <c r="C7" s="32"/>
+      <c r="D7" s="23">
         <v>1.2969999999999999</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="24">
+      <c r="F7" s="23">
         <v>2.6</v>
       </c>
-      <c r="G7" s="25">
+      <c r="G7" s="24">
         <v>8</v>
       </c>
       <c r="H7">
@@ -2753,20 +2775,20 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
+      <c r="B8" s="22">
         <v>43868.328472222223</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="24">
+      <c r="C8" s="32"/>
+      <c r="D8" s="23">
         <v>1.2669999999999999</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="F8" s="24">
+      <c r="F8" s="23">
         <v>3.532</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="24">
         <v>11</v>
       </c>
       <c r="H8">
@@ -2774,20 +2796,20 @@
       </c>
     </row>
     <row r="9" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23">
+      <c r="B9" s="22">
         <v>43868.259027777778</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="24">
+      <c r="C9" s="32"/>
+      <c r="D9" s="23">
         <v>0.94399999999999995</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="23">
         <v>4.1029999999999998</v>
       </c>
-      <c r="G9" s="25">
+      <c r="G9" s="24">
         <v>12</v>
       </c>
       <c r="H9">
@@ -2795,20 +2817,20 @@
       </c>
     </row>
     <row r="10" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23">
+      <c r="B10" s="22">
         <v>43869.338194444441</v>
       </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="24">
+      <c r="C10" s="32"/>
+      <c r="D10" s="23">
         <v>0.878</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="24">
+      <c r="F10" s="23">
         <v>2.8050000000000002</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="24">
         <v>9</v>
       </c>
       <c r="H10">
@@ -2816,20 +2838,20 @@
       </c>
     </row>
     <row r="11" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23">
+      <c r="B11" s="22">
         <v>43869.926388888889</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="24">
+      <c r="C11" s="32"/>
+      <c r="D11" s="23">
         <v>0.747</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F11" s="23">
         <v>1.0449999999999999</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="24">
         <v>6</v>
       </c>
       <c r="H11">
@@ -2837,20 +2859,20 @@
       </c>
     </row>
     <row r="12" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23">
+      <c r="B12" s="22">
         <v>43868.106249999997</v>
       </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="24">
+      <c r="C12" s="32"/>
+      <c r="D12" s="23">
         <v>0.63300000000000001</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="24">
+      <c r="F12" s="23">
         <v>2.9129999999999998</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="24">
         <v>10</v>
       </c>
       <c r="H12">
@@ -2858,20 +2880,20 @@
       </c>
     </row>
     <row r="13" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="19">
+      <c r="B13" s="18">
         <v>43870.665972222225</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="20">
+      <c r="C13" s="31"/>
+      <c r="D13" s="19">
         <v>0.63200000000000001</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="20">
+      <c r="F13" s="19">
         <v>0.51</v>
       </c>
-      <c r="G13" s="26">
+      <c r="G13" s="25">
         <v>4</v>
       </c>
       <c r="H13">
@@ -2879,20 +2901,20 @@
       </c>
     </row>
     <row r="14" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="19">
+      <c r="B14" s="18">
         <v>43860.736111111109</v>
       </c>
-      <c r="C14" s="34"/>
-      <c r="D14" s="20">
+      <c r="C14" s="31"/>
+      <c r="D14" s="19">
         <v>0.55500000000000005</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="20">
+      <c r="F14" s="19">
         <v>0.44700000000000001</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="25">
         <v>2</v>
       </c>
       <c r="H14">
@@ -2900,20 +2922,20 @@
       </c>
     </row>
     <row r="15" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="19">
+      <c r="B15" s="18">
         <v>43869.745833333334</v>
       </c>
-      <c r="C15" s="34"/>
-      <c r="D15" s="20">
+      <c r="C15" s="31"/>
+      <c r="D15" s="19">
         <v>0.51900000000000002</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="20">
+      <c r="F15" s="19">
         <v>0.38600000000000001</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="25">
         <v>1</v>
       </c>
       <c r="H15">
@@ -2921,20 +2943,20 @@
       </c>
     </row>
     <row r="16" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="19">
+      <c r="B16" s="18">
         <v>43869.500694444447</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="20">
+      <c r="C16" s="31"/>
+      <c r="D16" s="19">
         <v>0.51700000000000002</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="20">
+      <c r="F16" s="19">
         <v>0.49099999999999999</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="25">
         <v>3</v>
       </c>
       <c r="H16">
@@ -2942,20 +2964,20 @@
       </c>
     </row>
     <row r="17" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19">
+      <c r="B17" s="18">
         <v>43864.603472222225</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="20">
+      <c r="C17" s="31"/>
+      <c r="D17" s="19">
         <v>0.42799999999999999</v>
       </c>
-      <c r="E17" s="20">
+      <c r="E17" s="19">
         <v>1</v>
       </c>
-      <c r="F17" s="20">
+      <c r="F17" s="19">
         <v>0.85</v>
       </c>
-      <c r="G17" s="26">
+      <c r="G17" s="25">
         <v>5</v>
       </c>
       <c r="H17">
@@ -2975,327 +2997,389 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3C60E-DA9C-B543-9A00-6EBDC9C4D550}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="38" customWidth="1"/>
-    <col min="2" max="2" width="18.6640625" style="38" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="38"/>
-    <col min="4" max="4" width="10.83203125" style="41"/>
-    <col min="5" max="16384" width="10.83203125" style="38"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="38"/>
+      <c r="B2" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="37"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="39">
+      <c r="C2" s="38"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="33"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="34">
         <v>43868.520138888889</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="40">
+      <c r="C3" s="35">
         <v>3.3940000000000001</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="35">
         <v>1</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="35">
         <v>8.25</v>
       </c>
-      <c r="F3" s="38">
+      <c r="F3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="39">
+      <c r="G3">
+        <f>F3-D3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="34">
         <v>43871.665972222225</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="40">
+      <c r="C4" s="35">
         <v>2.6459999999999999</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="35">
         <v>2</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="35">
         <v>4.84</v>
       </c>
-      <c r="F4" s="38">
+      <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="39">
+      <c r="G4">
+        <f t="shared" ref="G4:G16" si="0">F4-D4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="34">
         <v>43869.433333333334</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="35">
         <v>1.3009999999999999</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="35">
         <v>3</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="35">
         <v>1.8520000000000001</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="39">
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="34">
         <v>43859.568749999999</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="40">
+      <c r="C6" s="35">
         <v>1.2969999999999999</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="35">
         <v>4</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="35">
         <v>2.6</v>
       </c>
-      <c r="F6" s="38">
+      <c r="F6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="39">
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="34">
         <v>43868.328472222223</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="40">
+      <c r="C7" s="35">
         <v>1.2669999999999999</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="35">
         <v>5</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="35">
         <v>3.532</v>
       </c>
-      <c r="F7" s="38">
+      <c r="F7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="39">
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="34">
         <v>43868.259027777778</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="40">
+      <c r="C8" s="35">
         <v>0.94399999999999995</v>
       </c>
-      <c r="D8" s="40">
+      <c r="D8" s="35">
         <v>6</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="35">
         <v>4.1029999999999998</v>
       </c>
-      <c r="F8" s="38">
+      <c r="F8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="39">
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="34">
         <v>43869.338194444441</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="40">
+      <c r="C9" s="35">
         <v>0.878</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="35">
         <v>7</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="35">
         <v>2.8050000000000002</v>
       </c>
-      <c r="F9" s="38">
+      <c r="F9">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="39">
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="34">
         <v>43869.926388888889</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="40">
+      <c r="C10" s="35">
         <v>0.747</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="35">
         <v>8</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="35">
         <v>1.0449999999999999</v>
       </c>
-      <c r="F10" s="38">
+      <c r="F10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="39">
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="34">
         <v>43868.106249999997</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="40">
+      <c r="C11" s="35">
         <v>0.63300000000000001</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="35">
         <v>9</v>
       </c>
-      <c r="E11" s="40">
+      <c r="E11" s="35">
         <v>2.9129999999999998</v>
       </c>
-      <c r="F11" s="38">
+      <c r="F11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="39">
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="34">
         <v>43870.665972222225</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="40">
+      <c r="C12" s="35">
         <v>0.63200000000000001</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="35">
         <v>10</v>
       </c>
-      <c r="E12" s="40">
+      <c r="E12" s="35">
         <v>0.51</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="39">
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="34">
         <v>43860.736111111109</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C13" s="35">
         <v>0.55500000000000005</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="35">
         <v>11</v>
       </c>
-      <c r="E13" s="40">
+      <c r="E13" s="35">
         <v>0.44700000000000001</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13">
         <v>13</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="39">
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="34">
         <v>43869.745833333334</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="40">
+      <c r="C14" s="35">
         <v>0.51900000000000002</v>
       </c>
-      <c r="D14" s="40">
+      <c r="D14" s="35">
         <v>12</v>
       </c>
-      <c r="E14" s="40">
+      <c r="E14" s="35">
         <v>0.38600000000000001</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14">
         <v>14</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="39">
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="34">
         <v>43869.500694444447</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="40">
+      <c r="C15" s="35">
         <v>0.51700000000000002</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="35">
         <v>13</v>
       </c>
-      <c r="E15" s="40">
+      <c r="E15" s="35">
         <v>0.49099999999999999</v>
       </c>
-      <c r="F15" s="38">
+      <c r="F15">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="39">
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="34">
         <v>43864.603472222225</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="40">
+      <c r="C16" s="35">
         <v>0.42799999999999999</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="35">
         <v>14</v>
       </c>
-      <c r="E16" s="40">
+      <c r="E16" s="35">
         <v>0.85</v>
       </c>
-      <c r="F16" s="38">
+      <c r="F16">
         <v>10</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.2">
+      <c r="G17" cm="1">
+        <f t="array" ref="G17">1 - 6*SUM((G3:G16)^2) / (14*14^2-1)</f>
+        <v>0.80751002551950424</v>
+      </c>
+      <c r="H17" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>